<commit_message>
Se agregó la funcionalidad de eliminar alumno
</commit_message>
<xml_diff>
--- a/reporte 1-9-2021.xlsx
+++ b/reporte 1-9-2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="92">
   <si>
     <t>Banco de Preguntas</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Dinastias</t>
   </si>
   <si>
-    <t>21322431-6</t>
-  </si>
-  <si>
     <t>32124222-1</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>log100 cos(x)</t>
   </si>
   <si>
-    <t>21000999-k</t>
-  </si>
-  <si>
     <t>Geometria</t>
   </si>
   <si>
@@ -291,7 +285,7 @@
     <t>Fuerzas</t>
   </si>
   <si>
-    <t>20999777-2</t>
+    <t>20789812-0</t>
   </si>
   <si>
     <t>Trigonometria</t>
@@ -300,7 +294,7 @@
     <t>CineYTeatro</t>
   </si>
   <si>
-    <t>23111444-2</t>
+    <t>12992231-k</t>
   </si>
 </sst>
 </file>
@@ -381,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -451,37 +445,37 @@
         <v>1.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="F3" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="H3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="K3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="M3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -489,40 +483,40 @@
         <v>34</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="E4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F4" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J4" t="n">
         <v>5.0</v>
       </c>
-      <c r="I4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.0</v>
-      </c>
       <c r="K4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="L4" t="n">
         <v>6.0</v>
       </c>
       <c r="M4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -530,13 +524,13 @@
         <v>35</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="n">
         <v>1.0</v>
@@ -545,25 +539,25 @@
         <v>3.0</v>
       </c>
       <c r="G5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I5" t="n">
         <v>5.0</v>
       </c>
-      <c r="H5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6.0</v>
-      </c>
       <c r="J5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K5" t="n">
         <v>2.0</v>
       </c>
       <c r="L5" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="M5" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -571,40 +565,40 @@
         <v>36</v>
       </c>
       <c r="B6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="n">
         <v>4.0</v>
       </c>
       <c r="D6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="E6" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="F6" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G6" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="H6" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="J6" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="K6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="L6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="M6" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -612,34 +606,34 @@
         <v>37</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J7" t="n">
         <v>5.0</v>
       </c>
-      <c r="E7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6.0</v>
-      </c>
       <c r="K7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="L7" t="n">
         <v>5.0</v>
@@ -648,140 +642,107 @@
         <v>4.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1.0</v>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>0</v>
+      <c r="A10" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="2">
-        <v>6</v>
+      <c r="A12" t="s" s="1">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="1">
-        <v>16</v>
+      <c r="A15" t="s" s="2">
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="2">
-        <v>21</v>
+      <c r="A17" t="s" s="1">
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="1">
-        <v>27</v>
+      <c r="A19" t="s" s="2">
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -789,25 +750,17 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -839,97 +792,97 @@
         <v>24</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>5.0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="H3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="I3" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="J3" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="G4" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I4" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="J4" t="n">
         <v>1.0</v>
@@ -937,98 +890,98 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C5" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F5" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G5" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I5" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="J5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="n">
         <v>2.0</v>
       </c>
       <c r="C6" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="E6" t="n">
         <v>2.0</v>
       </c>
       <c r="F6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H6" t="n">
         <v>5.0</v>
       </c>
-      <c r="G6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.0</v>
-      </c>
       <c r="I6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="J6" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="n">
         <v>4.0</v>
       </c>
       <c r="C7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="n">
         <v>3.0</v>
       </c>
       <c r="H7" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="I7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="J7" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
@@ -1038,7 +991,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1046,26 +999,26 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1073,7 +1026,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1081,7 +1034,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1089,7 +1042,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1097,7 +1050,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1105,16 +1058,16 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="4">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1145,24 +1098,24 @@
         <v>24</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>21</v>
@@ -1171,27 +1124,27 @@
         <v>18</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -1203,54 +1156,54 @@
         <v>4.0</v>
       </c>
       <c r="F3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="J3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="K3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="L3" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C4" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E4" t="n">
         <v>4.0</v>
       </c>
       <c r="F4" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="G4" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="J4" t="n">
         <v>6.0</v>
@@ -1259,39 +1212,39 @@
         <v>4.0</v>
       </c>
       <c r="L4" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C5" t="n">
         <v>5.0</v>
       </c>
-      <c r="C5" t="n">
-        <v>6.0</v>
-      </c>
       <c r="D5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E5" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="F5" t="n">
         <v>2.0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="H5" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="I5" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="J5" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="K5" t="n">
         <v>6.0</v>
@@ -1302,78 +1255,78 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I6" t="n">
         <v>5.0</v>
       </c>
-      <c r="F6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>6.0</v>
-      </c>
       <c r="J6" t="n">
         <v>2.0</v>
       </c>
       <c r="K6" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="L6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G7" t="n">
         <v>5.0</v>
       </c>
-      <c r="E7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.0</v>
-      </c>
       <c r="H7" t="n">
         <v>1.0</v>
       </c>
       <c r="I7" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="J7" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="K7" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="L7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -1383,7 +1336,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="6">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1391,7 +1344,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="6">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -1399,7 +1352,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="5">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1407,7 +1360,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="5">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1431,7 +1384,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="5">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1439,7 +1392,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="5">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1447,7 +1400,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="6">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -1455,7 +1408,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="6">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -1463,7 +1416,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="5">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -1488,32 +1441,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="D3" t="n">
         <v>6.0</v>
@@ -1526,7 +1479,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1534,7 +1487,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="7">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -1542,7 +1495,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="8">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -1569,15 +1522,12 @@
     </row>
     <row r="2">
       <c r="B2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6.0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -1587,10 +1537,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="10">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
         <v>79</v>
-      </c>
-      <c r="B6" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1618,30 +1568,30 @@
         <v>28</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="H2" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
@@ -1656,7 +1606,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="12">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1664,7 +1614,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="12">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -1672,7 +1622,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="11">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -1680,7 +1630,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="11">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1688,7 +1638,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="12">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1696,18 +1646,18 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="12">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
         <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="11">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1732,7 +1682,7 @@
     <row r="2"/>
     <row r="3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
@@ -1764,21 +1714,21 @@
     </row>
     <row r="2">
       <c r="B2" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -1788,7 +1738,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="16">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1796,7 +1746,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="15">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Se agrego la funcionalidad de modificar rut de Alumnos
</commit_message>
<xml_diff>
--- a/reporte 1-9-2021.xlsx
+++ b/reporte 1-9-2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="93">
   <si>
     <t>Banco de Preguntas</t>
   </si>
@@ -186,7 +186,7 @@
     <t>19321324-k</t>
   </si>
   <si>
-    <t>11241424-k</t>
+    <t>21312313-0</t>
   </si>
   <si>
     <t>20142252-1</t>
@@ -231,10 +231,10 @@
     <t>33243123-6</t>
   </si>
   <si>
-    <t>10023123-1</t>
-  </si>
-  <si>
-    <t>10000232-0</t>
+    <t>88888888-2</t>
+  </si>
+  <si>
+    <t>12449556-3</t>
   </si>
   <si>
     <t>31231223-6</t>
@@ -285,7 +285,10 @@
     <t>Fuerzas</t>
   </si>
   <si>
-    <t>20789812-0</t>
+    <t>24112232-0</t>
+  </si>
+  <si>
+    <t>20999122-2</t>
   </si>
   <si>
     <t>Trigonometria</t>
@@ -442,37 +445,37 @@
         <v>33</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H3" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="I3" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="L3" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="M3" t="n">
         <v>3.0</v>
@@ -483,40 +486,40 @@
         <v>34</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L4" t="n">
         <v>5.0</v>
       </c>
-      <c r="G4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>6.0</v>
-      </c>
       <c r="M4" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">
@@ -524,40 +527,40 @@
         <v>35</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C5" t="n">
         <v>5.0</v>
       </c>
       <c r="D5" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="H5" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I5" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="K5" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="L5" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="M5" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
@@ -565,40 +568,40 @@
         <v>36</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C6" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="F6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G6" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="H6" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="I6" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="J6" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="K6" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="L6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="M6" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -606,16 +609,16 @@
         <v>37</v>
       </c>
       <c r="B7" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
       <c r="D7" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n">
         <v>4.0</v>
@@ -624,22 +627,22 @@
         <v>3.0</v>
       </c>
       <c r="H7" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="I7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="J7" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="K7" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="L7" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M7" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
@@ -829,31 +832,31 @@
         <v>54</v>
       </c>
       <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E3" t="n">
         <v>5.0</v>
       </c>
-      <c r="C3" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.0</v>
-      </c>
       <c r="F3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I3" t="n">
         <v>6.0</v>
       </c>
       <c r="J3" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -861,31 +864,31 @@
         <v>55</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" t="n">
         <v>6.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F4" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="G4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="J4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -893,28 +896,28 @@
         <v>56</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" t="n">
         <v>4.0</v>
       </c>
       <c r="D5" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F5" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I5" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" t="n">
         <v>4.0</v>
@@ -925,31 +928,31 @@
         <v>57</v>
       </c>
       <c r="B6" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" t="n">
         <v>2.0</v>
       </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J6" t="n">
         <v>5.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -960,28 +963,28 @@
         <v>4.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E7" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="G7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="J7" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9">
@@ -1144,37 +1147,37 @@
         <v>69</v>
       </c>
       <c r="B3" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F3" t="n">
         <v>2.0</v>
       </c>
       <c r="G3" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I3" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="K3" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="L3" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="4">
@@ -1182,37 +1185,37 @@
         <v>70</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="I4" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="J4" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="K4" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="L4" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">
@@ -1223,34 +1226,34 @@
         <v>6.0</v>
       </c>
       <c r="C5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
         <v>5.0</v>
       </c>
-      <c r="D5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.0</v>
-      </c>
       <c r="G5" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="H5" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="I5" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="J5" t="n">
         <v>2.0</v>
       </c>
       <c r="K5" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
@@ -1258,37 +1261,37 @@
         <v>72</v>
       </c>
       <c r="B6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6" t="n">
         <v>5.0</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
-      </c>
       <c r="D6" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H6" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="I6" t="n">
         <v>5.0</v>
       </c>
       <c r="J6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K6" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="L6" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -1296,37 +1299,37 @@
         <v>73</v>
       </c>
       <c r="B7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F7" t="n">
         <v>5.0</v>
       </c>
-      <c r="C7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2.0</v>
-      </c>
       <c r="G7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J7" t="n">
         <v>5.0</v>
       </c>
-      <c r="H7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>3.0</v>
-      </c>
       <c r="K7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="L7" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
@@ -1463,13 +1466,13 @@
         <v>77</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5">
@@ -1670,7 +1673,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1685,8 +1688,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="4">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1714,21 +1722,21 @@
     </row>
     <row r="2">
       <c r="B2" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">
@@ -1738,7 +1746,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="16">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1746,7 +1754,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="15">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>

</xml_diff>